<commit_message>
hasta el dos de mayo
</commit_message>
<xml_diff>
--- a/mayo_02_2019_enviada.xlsx
+++ b/mayo_02_2019_enviada.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t xml:space="preserve">SISTEMA DE MONITORIZACIÓN DE MARIPOSAS</t>
   </si>
@@ -158,6 +158,13 @@
   </si>
   <si>
     <t xml:space="preserve">  NOTAS:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Han labrado la mitad del campo de almendros del tramo 3, y ademas lo han hecho con esos cacharros que lo dejan como harina ….. ,
+supongo que el proximo fin de semana labraran la otra mitad ….. un desastre </t>
+  </si>
+  <si>
+    <t xml:space="preserve">supongo que el proximo fin de semana labraran la otra mitad ….. un desastre </t>
   </si>
 </sst>
 </file>
@@ -172,11 +179,12 @@
     <numFmt numFmtId="168" formatCode="@"/>
     <numFmt numFmtId="169" formatCode="0.00"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -306,6 +314,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
@@ -693,8 +708,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -705,39 +720,39 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -824,9 +839,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>673560</xdr:colOff>
+      <xdr:colOff>673200</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>306720</xdr:rowOff>
+      <xdr:rowOff>306360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -835,8 +850,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12799440" y="12040560"/>
-          <a:ext cx="345240" cy="376200"/>
+          <a:off x="12800160" y="12040560"/>
+          <a:ext cx="344880" cy="375840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -893,9 +908,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>94320</xdr:colOff>
+      <xdr:colOff>93960</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>306720</xdr:rowOff>
+      <xdr:rowOff>306360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -904,8 +919,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5135760" y="11989080"/>
-          <a:ext cx="609840" cy="427680"/>
+          <a:off x="5136480" y="11989080"/>
+          <a:ext cx="609480" cy="427320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -962,9 +977,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>695160</xdr:colOff>
+      <xdr:colOff>694800</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>56160</xdr:rowOff>
+      <xdr:rowOff>55800</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -973,8 +988,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11028600" y="12006360"/>
-          <a:ext cx="2137680" cy="1351440"/>
+          <a:off x="11028960" y="12006360"/>
+          <a:ext cx="2137680" cy="1351080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1012,9 +1027,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>328320</xdr:colOff>
+      <xdr:colOff>327960</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>46440</xdr:rowOff>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1027,8 +1042,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11429640" y="12125160"/>
-          <a:ext cx="1369800" cy="1002600"/>
+          <a:off x="11430360" y="12125160"/>
+          <a:ext cx="1369440" cy="1002240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1049,9 +1064,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>485640</xdr:colOff>
+      <xdr:colOff>485280</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>44640</xdr:rowOff>
+      <xdr:rowOff>44280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1060,8 +1075,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="451800" y="11994840"/>
-          <a:ext cx="2385000" cy="1351440"/>
+          <a:off x="452520" y="11994840"/>
+          <a:ext cx="2384640" cy="1351080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1099,9 +1114,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1507680</xdr:colOff>
+      <xdr:colOff>1507320</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>196560</xdr:rowOff>
+      <xdr:rowOff>196200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1114,8 +1129,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="801000" y="12140280"/>
-          <a:ext cx="1032120" cy="917280"/>
+          <a:off x="801720" y="12140280"/>
+          <a:ext cx="1031760" cy="916920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1136,9 +1151,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>306000</xdr:colOff>
+      <xdr:colOff>305640</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>38880</xdr:rowOff>
+      <xdr:rowOff>38520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1147,8 +1162,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6101280" y="11989080"/>
-          <a:ext cx="2129400" cy="1351440"/>
+          <a:off x="6102000" y="11989080"/>
+          <a:ext cx="2129040" cy="1351080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1186,9 +1201,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>6840</xdr:colOff>
+      <xdr:colOff>6480</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>205920</xdr:rowOff>
+      <xdr:rowOff>205560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1201,8 +1216,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6363000" y="12118320"/>
-          <a:ext cx="1568520" cy="948600"/>
+          <a:off x="6363720" y="12118320"/>
+          <a:ext cx="1568160" cy="948240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1223,9 +1238,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>74160</xdr:colOff>
+      <xdr:colOff>73800</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1234,8 +1249,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3304080" y="12004200"/>
-          <a:ext cx="2421360" cy="1351440"/>
+          <a:off x="3304800" y="12004200"/>
+          <a:ext cx="2421000" cy="1351080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1273,9 +1288,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>588240</xdr:colOff>
+      <xdr:colOff>587880</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>175320</xdr:rowOff>
+      <xdr:rowOff>174960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1288,8 +1303,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3576240" y="12119040"/>
-          <a:ext cx="1526760" cy="917280"/>
+          <a:off x="3576960" y="12119040"/>
+          <a:ext cx="1526400" cy="916920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1310,9 +1325,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>729360</xdr:colOff>
+      <xdr:colOff>729000</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>83160</xdr:rowOff>
+      <xdr:rowOff>82800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1325,8 +1340,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4657680" y="12642120"/>
-          <a:ext cx="586440" cy="522360"/>
+          <a:off x="4658400" y="12642120"/>
+          <a:ext cx="586080" cy="522000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1347,9 +1362,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>445320</xdr:colOff>
+      <xdr:colOff>444960</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:rowOff>40320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1358,8 +1373,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8509680" y="11990880"/>
-          <a:ext cx="2133720" cy="1351440"/>
+          <a:off x="8510400" y="11990880"/>
+          <a:ext cx="2133000" cy="1351080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1397,9 +1412,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>70920</xdr:colOff>
+      <xdr:colOff>70560</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>77040</xdr:rowOff>
+      <xdr:rowOff>76680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1412,8 +1427,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8619480" y="12155760"/>
-          <a:ext cx="1649520" cy="1002600"/>
+          <a:off x="8620200" y="12155760"/>
+          <a:ext cx="1648800" cy="1002240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1434,9 +1449,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>92880</xdr:colOff>
+      <xdr:colOff>92520</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:rowOff>154080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1449,8 +1464,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9330120" y="12171240"/>
-          <a:ext cx="960840" cy="623880"/>
+          <a:off x="9330840" y="12171240"/>
+          <a:ext cx="960120" cy="623520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1471,9 +1486,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>465480</xdr:colOff>
+      <xdr:colOff>465120</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>292680</xdr:rowOff>
+      <xdr:rowOff>292320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1482,8 +1497,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2507760" y="12000600"/>
-          <a:ext cx="308880" cy="402120"/>
+          <a:off x="2508480" y="12000600"/>
+          <a:ext cx="308520" cy="401760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1540,9 +1555,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>274680</xdr:colOff>
+      <xdr:colOff>274320</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>306720</xdr:rowOff>
+      <xdr:rowOff>306360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1551,8 +1566,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7603920" y="11994840"/>
-          <a:ext cx="595440" cy="421920"/>
+          <a:off x="7604640" y="11994840"/>
+          <a:ext cx="595080" cy="421560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1609,9 +1624,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>419400</xdr:colOff>
+      <xdr:colOff>419040</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>2880</xdr:rowOff>
+      <xdr:rowOff>2520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1620,8 +1635,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10289520" y="12013920"/>
-          <a:ext cx="327960" cy="409320"/>
+          <a:off x="10289880" y="12013920"/>
+          <a:ext cx="327600" cy="408960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1679,13 +1694,13 @@
   </sheetPr>
   <dimension ref="A1:AMJ65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L66" activeCellId="0" sqref="L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="4" style="2" width="16.11"/>
@@ -2664,8 +2679,10 @@
       <c r="K51" s="49"/>
       <c r="L51" s="50"/>
     </row>
-    <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="51"/>
+    <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B52" s="51" t="s">
+        <v>46</v>
+      </c>
       <c r="C52" s="51"/>
       <c r="D52" s="51"/>
       <c r="E52" s="51"/>
@@ -2678,7 +2695,9 @@
       <c r="L52" s="51"/>
     </row>
     <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="51"/>
+      <c r="B53" s="51" t="s">
+        <v>47</v>
+      </c>
       <c r="C53" s="51"/>
       <c r="D53" s="51"/>
       <c r="E53" s="51"/>

</xml_diff>